<commit_message>
Added Excel module that generates points along the nosecone in a seperate sheet. The points are then plotted as a scatterplot to visualize the nosecone shape. Additionally, the macro uses the trapezoid rule to calculate the planform area of the nosecone.
</commit_message>
<xml_diff>
--- a/data/nosecones.xlsx
+++ b/data/nosecones.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Space\rocketry-performance\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Space\Documents\Emily\Rocketry_Performance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="731" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="731" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rocket" sheetId="10" r:id="rId1"/>
@@ -338,9 +338,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -534,18 +534,18 @@
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -558,29 +558,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -591,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -600,16 +600,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1541,11 +1541,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="465861056"/>
-        <c:axId val="465861448"/>
+        <c:axId val="426216152"/>
+        <c:axId val="426216544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="465861056"/>
+        <c:axId val="426216152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,12 +1619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465861448"/>
+        <c:crossAx val="426216544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="465861448"/>
+        <c:axId val="426216544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -1700,7 +1700,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465861056"/>
+        <c:crossAx val="426216152"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2665,11 +2665,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="465862232"/>
-        <c:axId val="465862624"/>
+        <c:axId val="426217328"/>
+        <c:axId val="426217720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="465862232"/>
+        <c:axId val="426217328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2743,12 +2743,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465862624"/>
+        <c:crossAx val="426217720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="465862624"/>
+        <c:axId val="426217720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -2824,7 +2824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465862232"/>
+        <c:crossAx val="426217328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3789,11 +3789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="465858704"/>
-        <c:axId val="465859096"/>
+        <c:axId val="426218504"/>
+        <c:axId val="426218896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="465858704"/>
+        <c:axId val="426218504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3867,12 +3867,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465859096"/>
+        <c:crossAx val="426218896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="465859096"/>
+        <c:axId val="426218896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -3948,7 +3948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465858704"/>
+        <c:crossAx val="426218504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4913,11 +4913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="465859880"/>
-        <c:axId val="465860272"/>
+        <c:axId val="427846832"/>
+        <c:axId val="427847224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="465859880"/>
+        <c:axId val="427846832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4991,12 +4991,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465860272"/>
+        <c:crossAx val="427847224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="465860272"/>
+        <c:axId val="427847224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -5072,7 +5072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="465859880"/>
+        <c:crossAx val="427846832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6511,15 +6511,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7002,10 +7002,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7030,10 +7031,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7171,13 +7173,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7215,10 +7217,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7562,7 +7565,7 @@
         <v>1.82</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
+        <f>0.5*$J$5*(1-((A21+J$9)/J$11)^J$8)*J$11^J$8/(J$11^J$8-J$9^J$8)</f>
         <v>1.9878114086146681</v>
       </c>
       <c r="C21" s="3">
@@ -8283,6 +8286,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9235,10 +9239,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10187,10 +10192,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>